<commit_message>
Ambito now recognize some vars, theres still some others elemets to save into db left, TODO: Count errors
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Matriz_Sintaxis.xlsx
+++ b/src/main/java/resources/Matriz_Sintaxis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\CompiladorAna\Compilador2024\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91293DA-E63D-49F3-B203-7D62F5344833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0DA1A-A479-4B96-AF1A-1CB36A182B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0B5114E-183A-43BB-9F44-9CB38DC39258}"/>
+    <workbookView xWindow="-28800" yWindow="-1725" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{C0B5114E-183A-43BB-9F44-9CB38DC39258}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz_Sintaxis" sheetId="1" r:id="rId1"/>
@@ -589,18 +589,12 @@
     <t>V1</t>
   </si>
   <si>
-    <t>PPAL⟶E1 { STATU E5 }</t>
-  </si>
-  <si>
     <t xml:space="preserve">E1⟶INTERF E1 </t>
   </si>
   <si>
     <t xml:space="preserve">E1⟶CLASE E1 </t>
   </si>
   <si>
-    <t xml:space="preserve">E1⟶LET E3 E4 </t>
-  </si>
-  <si>
     <t>E1⟶DEC_FUN E2</t>
   </si>
   <si>
@@ -616,9 +610,6 @@
     <t>E5⟶; STATU E5</t>
   </si>
   <si>
-    <t>CLASE⟶class id { DEC_VAR A1 DEC_MET A2 }</t>
-  </si>
-  <si>
     <t>A1⟶; DEC_VAR A1</t>
   </si>
   <si>
@@ -904,9 +895,6 @@
     <t>FUNCION⟶MET_CAD</t>
   </si>
   <si>
-    <t>DEC_FUN⟶function B1 ( B2 ) B4 { B5 }</t>
-  </si>
-  <si>
     <t>B1⟶id</t>
   </si>
   <si>
@@ -961,9 +949,6 @@
     <t>G2⟶TIPO G4</t>
   </si>
   <si>
-    <t>G2⟶ id = CONSTIPO</t>
-  </si>
-  <si>
     <t>G4⟶= CONSTIPO</t>
   </si>
   <si>
@@ -973,12 +958,6 @@
     <t>G3⟶( DEC_VAR B3 ) =&gt; STATU</t>
   </si>
   <si>
-    <t>G3⟶new Array &lt; G5 &gt; ( OR C1 )</t>
-  </si>
-  <si>
-    <t>G3⟶ [ G6 ]</t>
-  </si>
-  <si>
     <t>G5⟶ TIPO</t>
   </si>
   <si>
@@ -997,12 +976,6 @@
     <t>STATU⟶ if ( OR ) STATU S1</t>
   </si>
   <si>
-    <t>STATU⟶ switch ( OR ) { case OR : STATU S2 }</t>
-  </si>
-  <si>
-    <t>STATU⟶ { STATU V1 }</t>
-  </si>
-  <si>
     <t>STATU⟶ while ( OR ) STATU</t>
   </si>
   <si>
@@ -1063,9 +1036,6 @@
     <t>S7⟶ of</t>
   </si>
   <si>
-    <t>DEC_MET⟶ Method id ( B2 ) B4 { U1 }</t>
-  </si>
-  <si>
     <t>U1⟶ var DEC_VAR B3 ; U2</t>
   </si>
   <si>
@@ -1097,6 +1067,36 @@
   </si>
   <si>
     <t>G1⟶= G3</t>
+  </si>
+  <si>
+    <t>PPAL⟶E1 @crearAmbito { STATU E5 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>STATU⟶ @crearAmbito { STATU V1 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>CLASE⟶class id @crearAmbito { DEC_VAR A1 DEC_MET A2 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>DEC_FUN⟶function B1 ( B2 ) B4 @crearAmbito { B5 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>STATU⟶ switch ( OR ) @crearAmbito { case OR : STATU S2 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>G2⟶id = CONSTIPO</t>
+  </si>
+  <si>
+    <t>G3⟶ @decArr [ G6 ]</t>
+  </si>
+  <si>
+    <t>G3⟶ @decNewArr new Array &lt; G5 &gt; ( OR C1 )</t>
+  </si>
+  <si>
+    <t>DEC_MET⟶ Method @decMet id @crearAmbito ( @decPar B2 ) B4 { U1 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1⟶@decVar LET E3 E4 </t>
   </si>
 </sst>
 </file>
@@ -1513,8 +1513,8 @@
   <dimension ref="A1:DO68"/>
   <sheetViews>
     <sheetView topLeftCell="AE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BJ9" sqref="BJ9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BJ12" sqref="BJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25995,863 +25995,863 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C1D1BF-8449-460C-9DA2-7004DE2B6E73}">
   <dimension ref="A1:A170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>184</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="7" t="s">
-        <v>187</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>193</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75">
       <c r="A14" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75">
       <c r="A16" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75">
       <c r="A17" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75">
       <c r="A19" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75">
       <c r="A20" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75">
       <c r="A21" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75">
       <c r="A22" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75">
       <c r="A23" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75">
       <c r="A24" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75">
       <c r="A25" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75">
       <c r="A26" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75">
       <c r="A27" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75">
       <c r="A28" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75">
       <c r="A29" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75">
       <c r="A30" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75">
       <c r="A31" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75">
       <c r="A32" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75">
       <c r="A33" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75">
       <c r="A34" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75">
       <c r="A35" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75">
       <c r="A36" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75">
       <c r="A37" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75">
       <c r="A38" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75">
       <c r="A39" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75">
       <c r="A40" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75">
       <c r="A41" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75">
       <c r="A42" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75">
       <c r="A43" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75">
       <c r="A44" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75">
       <c r="A45" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75">
       <c r="A46" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75">
       <c r="A47" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75">
       <c r="A48" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75">
       <c r="A49" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75">
       <c r="A50" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75">
       <c r="A51" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75">
       <c r="A52" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75">
       <c r="A53" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75">
       <c r="A54" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75">
       <c r="A55" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75">
       <c r="A56" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75">
       <c r="A57" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75">
       <c r="A58" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75">
       <c r="A59" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75">
       <c r="A60" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75">
       <c r="A61" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75">
       <c r="A62" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75">
       <c r="A63" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75">
       <c r="A64" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75">
       <c r="A65" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15.75">
       <c r="A66" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15.75">
       <c r="A67" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15.75">
       <c r="A68" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15.75">
       <c r="A69" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75">
       <c r="A70" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75">
       <c r="A71" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75">
       <c r="A72" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75">
       <c r="A73" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75">
       <c r="A74" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15.75">
       <c r="A75" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15.75">
       <c r="A76" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15.75">
       <c r="A77" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15.75">
       <c r="A78" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15.75">
       <c r="A79" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15.75">
       <c r="A80" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15.75">
       <c r="A81" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15.75">
       <c r="A82" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15.75">
       <c r="A83" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15.75">
       <c r="A84" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15.75">
       <c r="A85" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.75">
       <c r="A86" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.75">
       <c r="A87" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.75">
       <c r="A88" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.75">
       <c r="A89" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75">
       <c r="A90" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.75">
       <c r="A91" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.75">
       <c r="A92" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.75">
       <c r="A93" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.75">
       <c r="A94" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.75">
       <c r="A95" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.75">
       <c r="A96" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.75">
       <c r="A97" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.75">
       <c r="A98" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.75">
       <c r="A99" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75">
       <c r="A100" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.75">
       <c r="A101" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15.75">
       <c r="A102" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15.75">
       <c r="A103" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.75">
       <c r="A104" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15.75">
       <c r="A105" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15.75">
       <c r="A106" s="7" t="s">
-        <v>289</v>
+        <v>347</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.75">
       <c r="A107" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75">
       <c r="A108" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.75">
       <c r="A109" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.75">
       <c r="A110" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.75">
       <c r="A111" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15.75">
       <c r="A112" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75">
       <c r="A113" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.75">
       <c r="A114" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.75">
       <c r="A115" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.75">
       <c r="A116" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.75">
       <c r="A117" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15.75">
       <c r="A118" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15.75">
       <c r="A119" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15.75">
       <c r="A120" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15.75">
       <c r="A121" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.75">
       <c r="A122" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.75">
       <c r="A123" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15.75">
       <c r="A124" s="7" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15.75">
       <c r="A125" s="7" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15.75">
       <c r="A126" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15.75">
       <c r="A127" s="7" t="s">
-        <v>308</v>
+        <v>349</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15.75">
       <c r="A128" s="7" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75">
       <c r="A129" s="7" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75">
       <c r="A130" s="7" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75">
       <c r="A131" s="7" t="s">
-        <v>312</v>
+        <v>351</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75">
       <c r="A132" s="7" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75">
       <c r="A133" s="7" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75">
       <c r="A134" s="7" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15.75">
       <c r="A135" s="7" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15.75">
       <c r="A136" s="7" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75">
       <c r="A137" s="7" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75">
       <c r="A138" s="7" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.75">
       <c r="A139" s="7" t="s">
-        <v>320</v>
+        <v>348</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.75">
       <c r="A140" s="7" t="s">
-        <v>321</v>
+        <v>345</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15.75">
       <c r="A141" s="7" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.75">
       <c r="A142" s="7" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.75">
       <c r="A143" s="7" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.75">
       <c r="A144" s="7" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15.75">
       <c r="A145" s="7" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15.75">
       <c r="A146" s="7" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15.75">
       <c r="A147" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15.75">
       <c r="A148" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15.75">
       <c r="A149" s="7" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75">
       <c r="A150" s="7" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15.75">
       <c r="A151" s="7" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15.75">
       <c r="A152" s="7" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15.75">
       <c r="A153" s="7" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15.75">
       <c r="A154" s="7" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15.75">
       <c r="A155" s="7" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15.75">
       <c r="A156" s="7" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15.75">
       <c r="A157" s="7" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15.75">
       <c r="A158" s="7" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15.75">
       <c r="A159" s="7" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15.75">
       <c r="A160" s="7" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75">
       <c r="A161" s="7" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.75">
       <c r="A162" s="7" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15.75">
       <c r="A163" s="7" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15.75">
       <c r="A164" s="7" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15.75">
       <c r="A165" s="7" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15.75">
       <c r="A166" s="7" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15.75">
       <c r="A167" s="7" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15.75">
       <c r="A168" s="7" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15.75">
       <c r="A169" s="7" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15.75">
       <c r="A170" s="7" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compiler now counts errors but needs more testing, check lexer error: assignments tokens not detected correclty. Added README
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Matriz_Sintaxis.xlsx
+++ b/src/main/java/resources/Matriz_Sintaxis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\CompiladorAna\Compilador2024\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0DA1A-A479-4B96-AF1A-1CB36A182B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A982D0D-B00F-4E1A-8586-3B58DFF0CC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-1725" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{C0B5114E-183A-43BB-9F44-9CB38DC39258}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C0B5114E-183A-43BB-9F44-9CB38DC39258}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz_Sintaxis" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>==</t>
   </si>
   <si>
-    <t>¡=</t>
-  </si>
-  <si>
     <t>===</t>
   </si>
   <si>
@@ -610,15 +607,9 @@
     <t>E5⟶; STATU E5</t>
   </si>
   <si>
-    <t>A1⟶; DEC_VAR A1</t>
-  </si>
-  <si>
     <t>A2⟶DEC_MET A2</t>
   </si>
   <si>
-    <t>INTERF⟶interface id { DEC_VAR A1 }</t>
-  </si>
-  <si>
     <t>DEC_VAR⟶id : TIPO</t>
   </si>
   <si>
@@ -898,18 +889,9 @@
     <t>B1⟶id</t>
   </si>
   <si>
-    <t>B2⟶DEC_VAR B3</t>
-  </si>
-  <si>
-    <t>B3⟶, DEC_VAR B3</t>
-  </si>
-  <si>
     <t>B4⟶: TIPO</t>
   </si>
   <si>
-    <t>B5⟶ var DEC_VAR B3 ; B6</t>
-  </si>
-  <si>
     <t>B5⟶ DEC_FUN B7 STATU V1</t>
   </si>
   <si>
@@ -937,15 +919,6 @@
     <t>N2⟶ , N1</t>
   </si>
   <si>
-    <t>LET⟶let id G1</t>
-  </si>
-  <si>
-    <t>LET⟶const id G1</t>
-  </si>
-  <si>
-    <t>LET⟶var id G1</t>
-  </si>
-  <si>
     <t>G2⟶TIPO G4</t>
   </si>
   <si>
@@ -1036,9 +1009,6 @@
     <t>S7⟶ of</t>
   </si>
   <si>
-    <t>U1⟶ var DEC_VAR B3 ; U2</t>
-  </si>
-  <si>
     <t>U1⟶ DEC_MET U3 STATU V1</t>
   </si>
   <si>
@@ -1069,34 +1039,64 @@
     <t>G1⟶= G3</t>
   </si>
   <si>
-    <t>PPAL⟶E1 @crearAmbito { STATU E5 } @eliminarAmbito</t>
-  </si>
-  <si>
-    <t>STATU⟶ @crearAmbito { STATU V1 } @eliminarAmbito</t>
-  </si>
-  <si>
-    <t>CLASE⟶class id @crearAmbito { DEC_VAR A1 DEC_MET A2 } @eliminarAmbito</t>
-  </si>
-  <si>
-    <t>DEC_FUN⟶function B1 ( B2 ) B4 @crearAmbito { B5 } @eliminarAmbito</t>
-  </si>
-  <si>
     <t>STATU⟶ switch ( OR ) @crearAmbito { case OR : STATU S2 } @eliminarAmbito</t>
   </si>
   <si>
     <t>G2⟶id = CONSTIPO</t>
   </si>
   <si>
-    <t>G3⟶ @decArr [ G6 ]</t>
-  </si>
-  <si>
-    <t>G3⟶ @decNewArr new Array &lt; G5 &gt; ( OR C1 )</t>
-  </si>
-  <si>
-    <t>DEC_MET⟶ Method @decMet id @crearAmbito ( @decPar B2 ) B4 { U1 } @eliminarAmbito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1⟶@decVar LET E3 E4 </t>
+    <t>A1⟶; @decVar2 DEC_VAR A1</t>
+  </si>
+  <si>
+    <t>B5⟶ var @decVar2 DEC_VAR B3 ; B6</t>
+  </si>
+  <si>
+    <t>U1⟶ var @decVar2 DEC_VAR B3 ; U2</t>
+  </si>
+  <si>
+    <t>CLASE⟶class @decInCa id @crearAmbito { @decVar2 DEC_VAR A1 DEC_MET A2 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>INTERF⟶interface @decInCa id @crearAmbito { @decVar2 DEC_VAR A1 } @eliminarAmbito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1⟶LET E3 E4 </t>
+  </si>
+  <si>
+    <t>LET⟶let @decVar id G1</t>
+  </si>
+  <si>
+    <t>LET⟶const @decVar id G1</t>
+  </si>
+  <si>
+    <t>LET⟶var @decVar id G1</t>
+  </si>
+  <si>
+    <t>G3⟶new Array &lt; G5 &gt; ( OR C1 )</t>
+  </si>
+  <si>
+    <t>G3⟶[ G6 ]</t>
+  </si>
+  <si>
+    <t>PPAL⟶E1 @crearAmbito @zonaEjec { STATU E5 } @zonaDec @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>DEC_FUN⟶function @decFun B1 @crearAmbito @parOn ( B2 ) @parOff B4  { B5 @zonaEjec } @zonaDec @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>DEC_MET⟶ Method @decMet id @crearAmbito @parOn ( B2 ) @parOff B4 { U1 @zonaEjec } @zonaDec @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>B2⟶@decVar2 DEC_VAR B3</t>
+  </si>
+  <si>
+    <t>B3⟶, @decVar2 DEC_VAR B3</t>
+  </si>
+  <si>
+    <t>STATU⟶ @crearAmbito @zonaEjec { STATU V1 } @zonaDec @eliminarAmbito</t>
+  </si>
+  <si>
+    <t>!=</t>
   </si>
 </sst>
 </file>
@@ -1512,9 +1512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814D01A7-BAB6-4E67-B147-60999809DA94}">
   <dimension ref="A1:DO68"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BJ12" sqref="BJ12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1654,283 +1654,283 @@
         <v>23</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DN1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:119">
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="4">
         <v>507</v>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="4">
         <v>508</v>
@@ -2656,7 +2656,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="4">
         <v>509</v>
@@ -3015,7 +3015,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="4">
         <v>510</v>
@@ -3374,7 +3374,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="4">
         <v>511</v>
@@ -3733,7 +3733,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="4">
         <v>512</v>
@@ -4092,7 +4092,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="4">
         <v>513</v>
@@ -4451,7 +4451,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="4">
         <v>514</v>
@@ -4810,7 +4810,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="4">
         <v>515</v>
@@ -5169,7 +5169,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="4">
         <v>516</v>
@@ -5528,7 +5528,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" s="4">
         <v>517</v>
@@ -5887,7 +5887,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="4">
         <v>518</v>
@@ -6246,7 +6246,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" s="4">
         <v>15</v>
@@ -6605,7 +6605,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" s="4">
         <v>520</v>
@@ -6964,7 +6964,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="4">
         <v>521</v>
@@ -7323,7 +7323,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="4">
         <v>522</v>
@@ -7682,7 +7682,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="4">
         <v>32</v>
@@ -8041,7 +8041,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="4">
         <v>524</v>
@@ -8400,7 +8400,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="4">
         <v>35</v>
@@ -8759,7 +8759,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="4">
         <v>526</v>
@@ -9118,7 +9118,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" s="4">
         <v>39</v>
@@ -9477,7 +9477,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="4">
         <v>528</v>
@@ -9836,7 +9836,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" s="4">
         <v>48</v>
@@ -10195,7 +10195,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C25" s="4">
         <v>530</v>
@@ -10554,7 +10554,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="4">
         <v>54</v>
@@ -10913,7 +10913,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="4">
         <v>532</v>
@@ -11272,7 +11272,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="4">
         <v>58</v>
@@ -11631,7 +11631,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="4">
         <v>534</v>
@@ -11990,7 +11990,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" s="4">
         <v>62</v>
@@ -12349,7 +12349,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C31" s="4">
         <v>536</v>
@@ -12708,7 +12708,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="4">
         <v>537</v>
@@ -13067,7 +13067,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="4">
         <v>71</v>
@@ -13426,7 +13426,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="4">
         <v>539</v>
@@ -13785,7 +13785,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="4">
         <v>540</v>
@@ -14144,7 +14144,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" s="4">
         <v>541</v>
@@ -14503,7 +14503,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="4">
         <v>542</v>
@@ -14862,7 +14862,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="4">
         <v>543</v>
@@ -15221,7 +15221,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C39" s="4">
         <v>544</v>
@@ -15580,7 +15580,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" s="4">
         <v>545</v>
@@ -15939,7 +15939,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C41" s="4">
         <v>546</v>
@@ -16298,7 +16298,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C42" s="4">
         <v>547</v>
@@ -16657,7 +16657,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="4">
         <v>112</v>
@@ -17016,7 +17016,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" s="4">
         <v>114</v>
@@ -17375,7 +17375,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C45" s="4">
         <v>169</v>
@@ -17734,7 +17734,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" s="4">
         <v>551</v>
@@ -18093,7 +18093,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C47" s="4">
         <v>552</v>
@@ -18452,7 +18452,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C48" s="4">
         <v>553</v>
@@ -18811,7 +18811,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" s="4">
         <v>554</v>
@@ -19170,7 +19170,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C50" s="4">
         <v>555</v>
@@ -19529,7 +19529,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C51" s="4">
         <v>556</v>
@@ -19888,7 +19888,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" s="4">
         <v>557</v>
@@ -20247,7 +20247,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" s="4">
         <v>558</v>
@@ -20606,7 +20606,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C54" s="4">
         <v>559</v>
@@ -20965,7 +20965,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" s="4">
         <v>134</v>
@@ -21324,7 +21324,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C56" s="4">
         <v>141</v>
@@ -21683,7 +21683,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C57" s="4">
         <v>562</v>
@@ -22042,7 +22042,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C58" s="4">
         <v>563</v>
@@ -22401,7 +22401,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C59" s="4">
         <v>564</v>
@@ -22760,7 +22760,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="4">
         <v>152</v>
@@ -23119,7 +23119,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="4">
         <v>154</v>
@@ -23478,7 +23478,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62" s="4">
         <v>156</v>
@@ -23837,7 +23837,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C63" s="4">
         <v>568</v>
@@ -24196,7 +24196,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C64" s="4">
         <v>569</v>
@@ -24555,7 +24555,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C65" s="4">
         <v>163</v>
@@ -24914,7 +24914,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C66" s="4">
         <v>165</v>
@@ -25273,7 +25273,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C67" s="4">
         <v>169</v>
@@ -25632,7 +25632,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C68" s="5">
         <v>573</v>
@@ -25995,863 +25995,863 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C1D1BF-8449-460C-9DA2-7004DE2B6E73}">
   <dimension ref="A1:A170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="145.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="7" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="7" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75">
       <c r="A5" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75">
       <c r="A6" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>191</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75">
       <c r="A13" s="7" t="s">
-        <v>193</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75">
       <c r="A14" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75">
       <c r="A15" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75">
       <c r="A16" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75">
       <c r="A17" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
       <c r="A18" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75">
       <c r="A19" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75">
       <c r="A20" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75">
       <c r="A21" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75">
       <c r="A22" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75">
       <c r="A23" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75">
       <c r="A24" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75">
       <c r="A25" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75">
       <c r="A26" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75">
       <c r="A27" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75">
       <c r="A28" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75">
       <c r="A29" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75">
       <c r="A30" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75">
       <c r="A31" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75">
       <c r="A32" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75">
       <c r="A33" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75">
       <c r="A34" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75">
       <c r="A35" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75">
       <c r="A36" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75">
       <c r="A37" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.75">
       <c r="A38" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.75">
       <c r="A39" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75">
       <c r="A40" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75">
       <c r="A41" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75">
       <c r="A42" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75">
       <c r="A43" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75">
       <c r="A44" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75">
       <c r="A45" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75">
       <c r="A46" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75">
       <c r="A47" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75">
       <c r="A48" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75">
       <c r="A49" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75">
       <c r="A50" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15.75">
       <c r="A51" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15.75">
       <c r="A52" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75">
       <c r="A53" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75">
       <c r="A54" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15.75">
       <c r="A55" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15.75">
       <c r="A56" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15.75">
       <c r="A57" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15.75">
       <c r="A58" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.75">
       <c r="A59" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75">
       <c r="A60" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75">
       <c r="A61" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75">
       <c r="A62" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.75">
       <c r="A63" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15.75">
       <c r="A64" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15.75">
       <c r="A65" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15.75">
       <c r="A66" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15.75">
       <c r="A67" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15.75">
       <c r="A68" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15.75">
       <c r="A69" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75">
       <c r="A70" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75">
       <c r="A71" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75">
       <c r="A72" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75">
       <c r="A73" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75">
       <c r="A74" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15.75">
       <c r="A75" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15.75">
       <c r="A76" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15.75">
       <c r="A77" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15.75">
       <c r="A78" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15.75">
       <c r="A79" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15.75">
       <c r="A80" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15.75">
       <c r="A81" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15.75">
       <c r="A82" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15.75">
       <c r="A83" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15.75">
       <c r="A84" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15.75">
       <c r="A85" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.75">
       <c r="A86" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.75">
       <c r="A87" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.75">
       <c r="A88" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.75">
       <c r="A89" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75">
       <c r="A90" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.75">
       <c r="A91" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.75">
       <c r="A92" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.75">
       <c r="A93" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.75">
       <c r="A94" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.75">
       <c r="A95" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.75">
       <c r="A96" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.75">
       <c r="A97" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.75">
       <c r="A98" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.75">
       <c r="A99" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.75">
       <c r="A100" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.75">
       <c r="A101" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15.75">
       <c r="A102" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15.75">
       <c r="A103" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.75">
       <c r="A104" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15.75">
       <c r="A105" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15.75">
       <c r="A106" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.75">
       <c r="A107" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.75">
       <c r="A108" s="7" t="s">
-        <v>287</v>
+        <v>350</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.75">
       <c r="A109" s="7" t="s">
-        <v>288</v>
+        <v>351</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.75">
       <c r="A110" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.75">
       <c r="A111" s="7" t="s">
-        <v>290</v>
+        <v>337</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15.75">
       <c r="A112" s="7" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75">
       <c r="A113" s="7" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.75">
       <c r="A114" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.75">
       <c r="A115" s="7" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.75">
       <c r="A116" s="7" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.75">
       <c r="A117" s="7" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15.75">
       <c r="A118" s="7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15.75">
       <c r="A119" s="7" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15.75">
       <c r="A120" s="7" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15.75">
       <c r="A121" s="7" t="s">
-        <v>300</v>
+        <v>342</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.75">
       <c r="A122" s="7" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.75">
       <c r="A123" s="7" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15.75">
       <c r="A124" s="7" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15.75">
       <c r="A125" s="7" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15.75">
       <c r="A126" s="7" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15.75">
       <c r="A127" s="7" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15.75">
       <c r="A128" s="7" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75">
       <c r="A129" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75">
       <c r="A130" s="7" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75">
       <c r="A131" s="7" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75">
       <c r="A132" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75">
       <c r="A133" s="7" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75">
       <c r="A134" s="7" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15.75">
       <c r="A135" s="7" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15.75">
       <c r="A136" s="7" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75">
       <c r="A137" s="7" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75">
       <c r="A138" s="7" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.75">
       <c r="A139" s="7" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.75">
       <c r="A140" s="7" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15.75">
       <c r="A141" s="7" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.75">
       <c r="A142" s="7" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.75">
       <c r="A143" s="7" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.75">
       <c r="A144" s="7" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15.75">
       <c r="A145" s="7" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15.75">
       <c r="A146" s="7" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15.75">
       <c r="A147" s="7" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15.75">
       <c r="A148" s="7" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15.75">
       <c r="A149" s="7" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75">
       <c r="A150" s="7" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15.75">
       <c r="A151" s="7" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15.75">
       <c r="A152" s="7" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15.75">
       <c r="A153" s="7" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15.75">
       <c r="A154" s="7" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15.75">
       <c r="A155" s="7" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15.75">
       <c r="A156" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15.75">
       <c r="A157" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15.75">
       <c r="A158" s="7" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15.75">
       <c r="A159" s="7" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15.75">
       <c r="A160" s="7" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75">
       <c r="A161" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.75">
       <c r="A162" s="7" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15.75">
       <c r="A163" s="7" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15.75">
       <c r="A164" s="7" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15.75">
       <c r="A165" s="7" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15.75">
       <c r="A166" s="7" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15.75">
       <c r="A167" s="7" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15.75">
       <c r="A168" s="7" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15.75">
       <c r="A169" s="7" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15.75">
       <c r="A170" s="7" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>